<commit_message>
Hoàn thiện AHP, fix UI, validate, chi tiết kết quả, CR từng bảng
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,11 +449,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tăng trưởng dài hạn</t>
+          <t>Ổn định giá</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.463932962529274</v>
+        <v>0.633345720302242</v>
       </c>
     </row>
     <row r="3">
@@ -463,27 +463,17 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2111026541764247</v>
+        <v>0.2604979561501301</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Khả năng chống lạm phát</t>
+          <t>Tăng trưởng dài hạn</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2628444574551132</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Rủi ro đầu tư</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.06211992583918813</v>
+        <v>0.1061563235476279</v>
       </c>
     </row>
   </sheetData>
@@ -497,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,11 +510,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Vàng</t>
+          <t>Ngoại tệ</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.25</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="3">
@@ -534,27 +524,17 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2401890673619175</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ngoại tệ</t>
+          <t>Vàng</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2305230538493319</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Trái phiếu</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.133924266726841</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>